<commit_message>
optimize method which get captcha from the website & auto delete img of captcha after analyse its code
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\little_trick\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876FC569-C71D-49FB-99B8-FC7129BE5583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D658B529-B5F7-4480-BC0B-E2D5BD758562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2352" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+  <si>
+    <t>newmaker.plus0@gmail.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>asd1016101610</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1050223@gm.yhsh.tn.edu.tw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>810002@gm.yhsh.tn.edu.tw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C14116132@gs.ncku.edu.tw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c14116132@gmail.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mr.871945@gmail.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -359,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -371,23 +400,64 @@
     <col min="2" max="2" width="30.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{20943097-CDB0-4772-823A-908264039E7E}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{AE929F0E-5A62-4810-AB81-1120C7241E03}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{A1C78FE8-162C-40CC-BDBB-D0C09F9A0F35}"/>
+    <hyperlink ref="A4" r:id="rId4" xr:uid="{B81D82A0-619B-4919-9366-2214129B1A03}"/>
+    <hyperlink ref="A5" r:id="rId5" xr:uid="{76892582-BD86-46BD-A8C6-3D0EA0EF7AEB}"/>
+    <hyperlink ref="A6" r:id="rId6" xr:uid="{6B5E882D-55F7-4D42-93A8-81904115CE04}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>